<commit_message>
Add JWT auth backend and update assets
</commit_message>
<xml_diff>
--- a/server/data/event_inquiries.xlsx
+++ b/server/data/event_inquiries.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -566,9 +566,50 @@
         <v/>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>2025-11-11T05:24:20.439Z</v>
+      </c>
+      <c r="B5" t="str">
+        <v>rrr</v>
+      </c>
+      <c r="C5" t="str">
+        <v>rrrry77</v>
+      </c>
+      <c r="D5" t="str">
+        <v>rry@gmail.co</v>
+      </c>
+      <c r="E5" t="str">
+        <v>+1 355 3456789</v>
+      </c>
+      <c r="F5" t="str">
+        <v>employer</v>
+      </c>
+      <c r="G5" t="str">
+        <v>dsefrr</v>
+      </c>
+      <c r="H5" t="str">
+        <v/>
+      </c>
+      <c r="I5" t="str">
+        <v/>
+      </c>
+      <c r="J5" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="K5">
+        <v>6</v>
+      </c>
+      <c r="L5" t="str">
+        <v>1113</v>
+      </c>
+      <c r="M5" t="str">
+        <v>gi</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:M4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:M5"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Finalize DataNexus assistant, docs, and port alignment
</commit_message>
<xml_diff>
--- a/server/data/event_inquiries.xlsx
+++ b/server/data/event_inquiries.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -607,9 +607,50 @@
         <v>gi</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>2025-11-14T04:32:20.098Z</v>
+      </c>
+      <c r="B6" t="str">
+        <v>de</v>
+      </c>
+      <c r="C6" t="str">
+        <v>eee</v>
+      </c>
+      <c r="D6" t="str">
+        <v>dev@gmail.com</v>
+      </c>
+      <c r="E6" t="str">
+        <v>3142977875</v>
+      </c>
+      <c r="F6" t="str">
+        <v>employer</v>
+      </c>
+      <c r="G6" t="str">
+        <v>efhf</v>
+      </c>
+      <c r="H6" t="str">
+        <v/>
+      </c>
+      <c r="I6" t="str">
+        <v/>
+      </c>
+      <c r="J6" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="K6">
+        <v>3</v>
+      </c>
+      <c r="L6" t="str">
+        <v>1140</v>
+      </c>
+      <c r="M6" t="str">
+        <v>def</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:M5"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:M6"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>